<commit_message>
Updates spreadsheets to remove duplicate bechdel test logging and Storm character visualizations
</commit_message>
<xml_diff>
--- a/spreadsheets/xmen_Bechdel_test.xlsx
+++ b/spreadsheets/xmen_Bechdel_test.xlsx
@@ -1,31 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sabrinawasserman/Workspace/The Claremont Run/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E36A945-DB31-D540-ABAD-25402C38E94C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38D19825-5EFA-DB46-B9B3-D5006BC7D972}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="27520" windowHeight="15560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="49">
   <si>
     <t>Issue #</t>
   </si>
@@ -62,15 +71,133 @@
   <si>
     <t>Notes</t>
   </si>
+  <si>
+    <t>Issues</t>
+  </si>
+  <si>
+    <t>Every 10 issues pass #  (out of 10)</t>
+  </si>
+  <si>
+    <t>1 -&gt; 10</t>
+  </si>
+  <si>
+    <t>11 -&gt;20</t>
+  </si>
+  <si>
+    <t>21 -&gt;30</t>
+  </si>
+  <si>
+    <t>31 -&gt;40</t>
+  </si>
+  <si>
+    <t>41 -&gt;50</t>
+  </si>
+  <si>
+    <t>51 -&gt;60</t>
+  </si>
+  <si>
+    <t>61 -&gt;70</t>
+  </si>
+  <si>
+    <t>71-&gt;80</t>
+  </si>
+  <si>
+    <t>81-&gt;90</t>
+  </si>
+  <si>
+    <t>91-&gt;100</t>
+  </si>
+  <si>
+    <t>101-110</t>
+  </si>
+  <si>
+    <t>111-120</t>
+  </si>
+  <si>
+    <t>121-130</t>
+  </si>
+  <si>
+    <t>131-140</t>
+  </si>
+  <si>
+    <t>141-&gt;150</t>
+  </si>
+  <si>
+    <t>151-&gt;160</t>
+  </si>
+  <si>
+    <t>161-&gt;170</t>
+  </si>
+  <si>
+    <t>171-&gt;180</t>
+  </si>
+  <si>
+    <t>181-&gt;190</t>
+  </si>
+  <si>
+    <t>191-&gt;200</t>
+  </si>
+  <si>
+    <t>201-&gt;210</t>
+  </si>
+  <si>
+    <t>211-&gt;220</t>
+  </si>
+  <si>
+    <t>221-&gt;230</t>
+  </si>
+  <si>
+    <t>231-&gt;340</t>
+  </si>
+  <si>
+    <t>241-&gt;250</t>
+  </si>
+  <si>
+    <t>251-&gt;260</t>
+  </si>
+  <si>
+    <t>261-&gt;270</t>
+  </si>
+  <si>
+    <t>271-&gt;280</t>
+  </si>
+  <si>
+    <t>281-&gt;290</t>
+  </si>
+  <si>
+    <t>291-&gt;300</t>
+  </si>
+  <si>
+    <t>301-&gt;310</t>
+  </si>
+  <si>
+    <t>311-&gt;320</t>
+  </si>
+  <si>
+    <t>321-&gt;330</t>
+  </si>
+  <si>
+    <t>331-&gt;340</t>
+  </si>
+  <si>
+    <t>341-&gt;350</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -96,8 +223,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -113,6 +243,1899 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Bechdel Test Pass Rate</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Per</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t> 10 issues of Uncanny X-Men (1963)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Every 10 issues pass #  (out of 10)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:marker>
+              <c:symbol val="none"/>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln w="28575" cap="rnd">
+                <a:solidFill>
+                  <a:srgbClr val="C00000"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-2D04-FE4D-A2FD-D17B6178A9AE}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:marker>
+              <c:symbol val="none"/>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln w="28575" cap="rnd">
+                <a:solidFill>
+                  <a:srgbClr val="C00000"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-2D04-FE4D-A2FD-D17B6178A9AE}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:marker>
+              <c:symbol val="none"/>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln w="28575" cap="rnd">
+                <a:solidFill>
+                  <a:srgbClr val="C00000"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-2D04-FE4D-A2FD-D17B6178A9AE}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="10"/>
+            <c:marker>
+              <c:symbol val="none"/>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln w="28575" cap="rnd">
+                <a:solidFill>
+                  <a:srgbClr val="C00000"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-2D04-FE4D-A2FD-D17B6178A9AE}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$D$2:$D$36</c:f>
+              <c:strCache>
+                <c:ptCount val="35"/>
+                <c:pt idx="0">
+                  <c:v>1 -&gt; 10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11 -&gt;20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21 -&gt;30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>31 -&gt;40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41 -&gt;50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>51 -&gt;60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>61 -&gt;70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>71-&gt;80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>81-&gt;90</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>91-&gt;100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>101-110</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>111-120</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>121-130</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>131-140</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>141-&gt;150</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>151-&gt;160</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>161-&gt;170</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>171-&gt;180</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>181-&gt;190</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>191-&gt;200</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>201-&gt;210</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>211-&gt;220</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>221-&gt;230</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>231-&gt;340</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>241-&gt;250</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>251-&gt;260</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>261-&gt;270</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>271-&gt;280</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>281-&gt;290</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>291-&gt;300</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>301-&gt;310</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>311-&gt;320</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>321-&gt;330</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>331-&gt;340</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>341-&gt;350</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$36</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="35"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2D04-FE4D-A2FD-D17B6178A9AE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="959044607"/>
+        <c:axId val="1009294111"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="959044607"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1100" b="0" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Issue Ranges (Inclusive)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-CA" sz="1100">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1009294111"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1009294111"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>% Issues Passed</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="959044607"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId3"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>129987</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>22412</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>44076</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>150905</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB094DA9-1E8F-8347-9112-43C4238B809B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.08515</cdr:x>
+      <cdr:y>0.93849</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.38901</cdr:x>
+      <cdr:y>1</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{776BE044-FDB2-7846-AD89-D7D7477DA470}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="965947" y="5819186"/>
+          <a:ext cx="3446987" cy="381401"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="800"/>
+            <a:t>= Includes reprinted</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="800" baseline="0"/>
+            <a:t> issues </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="800"/>
+            <a:t>(Issues</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="800" baseline="0"/>
+            <a:t> 67-93 are reprints of previous Uncanncy X-Men Issues)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="800"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.07063</cdr:x>
+      <cdr:y>0.94375</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.08643</cdr:x>
+      <cdr:y>0.97006</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="Oval 2">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2574556F-18CC-E042-9396-17F581B464F3}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="802336" y="5972857"/>
+          <a:ext cx="179464" cy="166527"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:srgbClr val="C00000"/>
+        </a:solidFill>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </cdr:style>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Characters"/>
+      <sheetName val="Locations"/>
+      <sheetName val="Covers"/>
+      <sheetName val="Bechdel Test"/>
+      <sheetName val="Covers Field Descriptions Rules"/>
+      <sheetName val="Field Descriptions"/>
+      <sheetName val="General Rules"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3">
+        <row r="1">
+          <cell r="F1" t="str">
+            <v>Every 10 issues pass #  (out of 10)</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="E2" t="str">
+            <v>1 -&gt; 10</v>
+          </cell>
+          <cell r="F2">
+            <v>0.1</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="E3" t="str">
+            <v>11 -&gt;20</v>
+          </cell>
+          <cell r="F3">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="E4" t="str">
+            <v>21 -&gt;30</v>
+          </cell>
+          <cell r="F4">
+            <v>0.1</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="E5" t="str">
+            <v>31 -&gt;40</v>
+          </cell>
+          <cell r="F5">
+            <v>0.1</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="E6" t="str">
+            <v>41 -&gt;50</v>
+          </cell>
+          <cell r="F6">
+            <v>0.1</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="E7" t="str">
+            <v>51 -&gt;60</v>
+          </cell>
+          <cell r="F7">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="E8" t="str">
+            <v>61 -&gt;70</v>
+          </cell>
+          <cell r="F8">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="E9" t="str">
+            <v>71-&gt;80</v>
+          </cell>
+          <cell r="F9">
+            <v>0.1</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="E10" t="str">
+            <v>81-&gt;90</v>
+          </cell>
+          <cell r="F10">
+            <v>0.1</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="E11" t="str">
+            <v>91-&gt;100</v>
+          </cell>
+          <cell r="F11">
+            <v>0.4</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="E12" t="str">
+            <v>101-110</v>
+          </cell>
+          <cell r="F12">
+            <v>0.6</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="E13" t="str">
+            <v>111-120</v>
+          </cell>
+          <cell r="F13">
+            <v>0.4</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="E14" t="str">
+            <v>121-130</v>
+          </cell>
+          <cell r="F14">
+            <v>0.5</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="E15" t="str">
+            <v>131-140</v>
+          </cell>
+          <cell r="F15">
+            <v>0.6</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="E16" t="str">
+            <v>141-&gt;150</v>
+          </cell>
+          <cell r="F16">
+            <v>0.8</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="E17" t="str">
+            <v>151-&gt;160</v>
+          </cell>
+          <cell r="F17">
+            <v>0.9</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="E18" t="str">
+            <v>161-&gt;170</v>
+          </cell>
+          <cell r="F18">
+            <v>0.8</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="E19" t="str">
+            <v>171-&gt;180</v>
+          </cell>
+          <cell r="F19">
+            <v>0.9</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="E20" t="str">
+            <v>181-&gt;190</v>
+          </cell>
+          <cell r="F20">
+            <v>0.8</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="E21" t="str">
+            <v>191-&gt;200</v>
+          </cell>
+          <cell r="F21">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="E22" t="str">
+            <v>201-&gt;210</v>
+          </cell>
+          <cell r="F22">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="E23" t="str">
+            <v>211-&gt;220</v>
+          </cell>
+          <cell r="F23">
+            <v>0.9</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="E24" t="str">
+            <v>221-&gt;230</v>
+          </cell>
+          <cell r="F24">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="E25" t="str">
+            <v>231-&gt;340</v>
+          </cell>
+          <cell r="F25">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="E26" t="str">
+            <v>241-&gt;250</v>
+          </cell>
+          <cell r="F26">
+            <v>0.9</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="E27" t="str">
+            <v>251-&gt;260</v>
+          </cell>
+          <cell r="F27">
+            <v>0.8</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="E28" t="str">
+            <v>261-&gt;270</v>
+          </cell>
+          <cell r="F28">
+            <v>0.9</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="E29" t="str">
+            <v>271-&gt;280</v>
+          </cell>
+          <cell r="F29">
+            <v>0.7</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="E30" t="str">
+            <v>281-&gt;290</v>
+          </cell>
+          <cell r="F30">
+            <v>0.4</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="E31" t="str">
+            <v>291-&gt;300</v>
+          </cell>
+          <cell r="F31">
+            <v>0.2</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="E32" t="str">
+            <v>301-&gt;310</v>
+          </cell>
+          <cell r="F32">
+            <v>0.4</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="E33" t="str">
+            <v>311-&gt;320</v>
+          </cell>
+          <cell r="F33">
+            <v>0.8</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="E34" t="str">
+            <v>321-&gt;330</v>
+          </cell>
+          <cell r="F34">
+            <v>0.4</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="E35" t="str">
+            <v>331-&gt;340</v>
+          </cell>
+          <cell r="F35">
+            <v>0.2</v>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="E36" t="str">
+            <v>341-&gt;350</v>
+          </cell>
+          <cell r="F36">
+            <v>0.3</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -378,19 +2401,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C546"/>
+  <dimension ref="A1:E546"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="D16" zoomScale="75" workbookViewId="0">
+      <selection activeCell="R41" sqref="R41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="51.83203125" customWidth="1"/>
+    <col min="4" max="4" width="14.5" customWidth="1"/>
+    <col min="5" max="5" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -400,288 +2425,504 @@
       <c r="C1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E20" s="3">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D21" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E21" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E22" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D23" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" s="3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D24" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E24" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D25" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E25" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E26" s="3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D27" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E27" s="3">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D28" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E28" s="3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D29" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E29" s="3">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D30" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E30" s="3">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D31" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E31" s="3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D32" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E32" s="3">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D33" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E33" s="3">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D34" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E34" s="3">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D35" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E35" s="3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D36" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E36" s="3">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -689,7 +2930,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -697,7 +2938,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -705,7 +2946,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -713,7 +2954,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -721,7 +2962,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -729,7 +2970,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -737,7 +2978,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -745,7 +2986,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -753,7 +2994,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -761,7 +3002,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -769,7 +3010,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -4772,5 +7013,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updates spreadsheets on site
</commit_message>
<xml_diff>
--- a/spreadsheets/xmen_Bechdel_test.xlsx
+++ b/spreadsheets/xmen_Bechdel_test.xlsx
@@ -1,40 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sabrinawasserman/Workspace/The Claremont Run/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38D19825-5EFA-DB46-B9B3-D5006BC7D972}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DD9770AF-F076-8C4A-8EAD-D51C7CB85C20}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="27520" windowHeight="15560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24680" windowHeight="15140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="85">
   <si>
     <t>Issue #</t>
   </si>
@@ -182,12 +175,120 @@
   <si>
     <t>341-&gt;350</t>
   </si>
+  <si>
+    <t>Penciller Collaborations</t>
+  </si>
+  <si>
+    <t>John Byrne</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>108-109, 111-142</t>
+  </si>
+  <si>
+    <t>Dave Cockrum</t>
+  </si>
+  <si>
+    <t>97-105, 107, 145-164</t>
+  </si>
+  <si>
+    <t>Percentage Passed</t>
+  </si>
+  <si>
+    <t>Paul Smith</t>
+  </si>
+  <si>
+    <t>165-170, 172-175, 278</t>
+  </si>
+  <si>
+    <t>John Romita Jr.</t>
+  </si>
+  <si>
+    <t>175-185, 187-197, 199-200, 202-203, 206-211</t>
+  </si>
+  <si>
+    <t>Marc Silvestri</t>
+  </si>
+  <si>
+    <t>Jim Lee</t>
+  </si>
+  <si>
+    <t>218, 220-222, 224-227, 229-230, 232-234, 236, 238-244, 246-247, 249-251, 253-255, 259-261</t>
+  </si>
+  <si>
+    <t>248, 256-258, 267-277</t>
+  </si>
+  <si>
+    <t>Marv Wolfman</t>
+  </si>
+  <si>
+    <t>Archie Goodwin</t>
+  </si>
+  <si>
+    <t>Jim Shooter</t>
+  </si>
+  <si>
+    <t>Tom Defalco</t>
+  </si>
+  <si>
+    <t>Editor Collaborations</t>
+  </si>
+  <si>
+    <t>Editor in Chief Collaborations</t>
+  </si>
+  <si>
+    <t>Roger Stern</t>
+  </si>
+  <si>
+    <t>Jim Salicrup</t>
+  </si>
+  <si>
+    <t>Louise Simonson</t>
+  </si>
+  <si>
+    <t>Ann Nocenti</t>
+  </si>
+  <si>
+    <t>Bob Harras</t>
+  </si>
+  <si>
+    <t>97-100</t>
+  </si>
+  <si>
+    <t>101-111</t>
+  </si>
+  <si>
+    <t>112-222</t>
+  </si>
+  <si>
+    <t>223-279</t>
+  </si>
+  <si>
+    <t>113-131</t>
+  </si>
+  <si>
+    <t>132-137</t>
+  </si>
+  <si>
+    <t>137-182</t>
+  </si>
+  <si>
+    <t>179-232</t>
+  </si>
+  <si>
+    <t>232-279</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,6 +303,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -211,7 +320,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -219,15 +328,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -681,11 +808,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="959044607"/>
-        <c:axId val="1009294111"/>
+        <c:axId val="151990056"/>
+        <c:axId val="151988880"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="959044607"/>
+        <c:axId val="151990056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -788,7 +915,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1009294111"/>
+        <c:crossAx val="151988880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -796,7 +923,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1009294111"/>
+        <c:axId val="151988880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -902,7 +1029,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="959044607"/>
+        <c:crossAx val="151990056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -959,7 +1086,1077 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="104"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="4"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="15"/>
+      <c:rotY val="20"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="1"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Percentage Passed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet3!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>John Byrne</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Dave Cockrum</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Paul Smith</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>John Romita Jr.</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Marc Silvestri</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Jim Lee</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$B$2:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>93</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E777-CD46-A6C8-1C080DBA572D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:shape val="box"/>
+        <c:axId val="325450776"/>
+        <c:axId val="325453912"/>
+        <c:axId val="0"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="325450776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="325453912"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="325453912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="325450776"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="15"/>
+      <c:rotY val="20"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="1"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$B$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Percentage Passed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet3!$A$10:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Marv Wolfman</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Archie Goodwin</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Jim Shooter</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Tom Defalco</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$B$10:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>89</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D32F-8B40-BEC0-64AB0E11AA16}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:shape val="box"/>
+        <c:axId val="392495960"/>
+        <c:axId val="392494392"/>
+        <c:axId val="0"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="392495960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="392494392"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="392494392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="392495960"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="15"/>
+      <c:rotY val="20"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="1"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$B$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Percentage Passed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet3!$A$16:$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Roger Stern</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Jim Salicrup</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Louise Simonson</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Ann Nocenti</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Bob Harras</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$B$16:$B$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>87</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4ED2-9F4B-9971-6D9A2D4363F2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:shape val="box"/>
+        <c:axId val="391245856"/>
+        <c:axId val="391247424"/>
+        <c:axId val="0"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="391245856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="391247424"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="391247424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="391245856"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinearReversed" id="22">
+  <a:schemeClr val="accent2"/>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1483,6 +2680,1488 @@
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -1827,315 +4506,117 @@
 </c:userShapes>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Characters"/>
-      <sheetName val="Locations"/>
-      <sheetName val="Covers"/>
-      <sheetName val="Bechdel Test"/>
-      <sheetName val="Covers Field Descriptions Rules"/>
-      <sheetName val="Field Descriptions"/>
-      <sheetName val="General Rules"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3">
-        <row r="1">
-          <cell r="F1" t="str">
-            <v>Every 10 issues pass #  (out of 10)</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="E2" t="str">
-            <v>1 -&gt; 10</v>
-          </cell>
-          <cell r="F2">
-            <v>0.1</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="E3" t="str">
-            <v>11 -&gt;20</v>
-          </cell>
-          <cell r="F3">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="E4" t="str">
-            <v>21 -&gt;30</v>
-          </cell>
-          <cell r="F4">
-            <v>0.1</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="E5" t="str">
-            <v>31 -&gt;40</v>
-          </cell>
-          <cell r="F5">
-            <v>0.1</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="E6" t="str">
-            <v>41 -&gt;50</v>
-          </cell>
-          <cell r="F6">
-            <v>0.1</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="E7" t="str">
-            <v>51 -&gt;60</v>
-          </cell>
-          <cell r="F7">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="E8" t="str">
-            <v>61 -&gt;70</v>
-          </cell>
-          <cell r="F8">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="E9" t="str">
-            <v>71-&gt;80</v>
-          </cell>
-          <cell r="F9">
-            <v>0.1</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="E10" t="str">
-            <v>81-&gt;90</v>
-          </cell>
-          <cell r="F10">
-            <v>0.1</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="E11" t="str">
-            <v>91-&gt;100</v>
-          </cell>
-          <cell r="F11">
-            <v>0.4</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="E12" t="str">
-            <v>101-110</v>
-          </cell>
-          <cell r="F12">
-            <v>0.6</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="E13" t="str">
-            <v>111-120</v>
-          </cell>
-          <cell r="F13">
-            <v>0.4</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="E14" t="str">
-            <v>121-130</v>
-          </cell>
-          <cell r="F14">
-            <v>0.5</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="E15" t="str">
-            <v>131-140</v>
-          </cell>
-          <cell r="F15">
-            <v>0.6</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="E16" t="str">
-            <v>141-&gt;150</v>
-          </cell>
-          <cell r="F16">
-            <v>0.8</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="E17" t="str">
-            <v>151-&gt;160</v>
-          </cell>
-          <cell r="F17">
-            <v>0.9</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="E18" t="str">
-            <v>161-&gt;170</v>
-          </cell>
-          <cell r="F18">
-            <v>0.8</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="E19" t="str">
-            <v>171-&gt;180</v>
-          </cell>
-          <cell r="F19">
-            <v>0.9</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="E20" t="str">
-            <v>181-&gt;190</v>
-          </cell>
-          <cell r="F20">
-            <v>0.8</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="E21" t="str">
-            <v>191-&gt;200</v>
-          </cell>
-          <cell r="F21">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="E22" t="str">
-            <v>201-&gt;210</v>
-          </cell>
-          <cell r="F22">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="E23" t="str">
-            <v>211-&gt;220</v>
-          </cell>
-          <cell r="F23">
-            <v>0.9</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="E24" t="str">
-            <v>221-&gt;230</v>
-          </cell>
-          <cell r="F24">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="E25" t="str">
-            <v>231-&gt;340</v>
-          </cell>
-          <cell r="F25">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="E26" t="str">
-            <v>241-&gt;250</v>
-          </cell>
-          <cell r="F26">
-            <v>0.9</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="E27" t="str">
-            <v>251-&gt;260</v>
-          </cell>
-          <cell r="F27">
-            <v>0.8</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="E28" t="str">
-            <v>261-&gt;270</v>
-          </cell>
-          <cell r="F28">
-            <v>0.9</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="E29" t="str">
-            <v>271-&gt;280</v>
-          </cell>
-          <cell r="F29">
-            <v>0.7</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="E30" t="str">
-            <v>281-&gt;290</v>
-          </cell>
-          <cell r="F30">
-            <v>0.4</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="E31" t="str">
-            <v>291-&gt;300</v>
-          </cell>
-          <cell r="F31">
-            <v>0.2</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="E32" t="str">
-            <v>301-&gt;310</v>
-          </cell>
-          <cell r="F32">
-            <v>0.4</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="E33" t="str">
-            <v>311-&gt;320</v>
-          </cell>
-          <cell r="F33">
-            <v>0.8</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="E34" t="str">
-            <v>321-&gt;330</v>
-          </cell>
-          <cell r="F34">
-            <v>0.4</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="E35" t="str">
-            <v>331-&gt;340</v>
-          </cell>
-          <cell r="F35">
-            <v>0.2</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="E36" t="str">
-            <v>341-&gt;350</v>
-          </cell>
-          <cell r="F36">
-            <v>0.3</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2403,8 +4884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E546"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D16" zoomScale="75" workbookViewId="0">
-      <selection activeCell="R41" sqref="R41"/>
+    <sheetView zoomScale="75" workbookViewId="0">
+      <selection activeCell="C246" sqref="C246"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7015,4 +9496,494 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15:E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="28.1640625" customWidth="1"/>
+    <col min="2" max="2" width="80.33203125" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2">
+        <v>20</v>
+      </c>
+      <c r="D2">
+        <v>15</v>
+      </c>
+      <c r="E2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3">
+        <v>23</v>
+      </c>
+      <c r="D3">
+        <v>7</v>
+      </c>
+      <c r="E3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5">
+        <v>30</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6">
+        <v>30</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7">
+        <v>10</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11">
+        <v>6</v>
+      </c>
+      <c r="D11">
+        <v>5</v>
+      </c>
+      <c r="E11">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C12">
+        <v>88</v>
+      </c>
+      <c r="D12">
+        <v>23</v>
+      </c>
+      <c r="E12">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C13">
+        <v>51</v>
+      </c>
+      <c r="D13">
+        <v>6</v>
+      </c>
+      <c r="E13">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B16" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16">
+        <v>10</v>
+      </c>
+      <c r="D16">
+        <v>9</v>
+      </c>
+      <c r="E16">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" t="s">
+        <v>81</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="E17">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18">
+        <v>37</v>
+      </c>
+      <c r="D18">
+        <v>9</v>
+      </c>
+      <c r="E18">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" t="s">
+        <v>83</v>
+      </c>
+      <c r="C19">
+        <v>51</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
+      </c>
+      <c r="E19">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>75</v>
+      </c>
+      <c r="B20" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20">
+        <v>42</v>
+      </c>
+      <c r="D20">
+        <v>6</v>
+      </c>
+      <c r="E20">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:B20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O18" sqref="O18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="34.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B16">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>75</v>
+      </c>
+      <c r="B20">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>